<commit_message>
Updte xlsx for topology
</commit_message>
<xml_diff>
--- a/doc/list_descriptor.xlsx
+++ b/doc/list_descriptor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borrela2\development\molecular-descriptors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8A5338-CBE7-4101-8D80-5F5517D2EF74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6FDBFE-5E1C-426D-B4C3-0ACC6B5AEFA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5295" yWindow="2460" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{6639A6CF-FE55-4264-9D0B-EE9D09DD7593}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="137">
   <si>
     <t>Constitutional</t>
   </si>
@@ -408,6 +408,42 @@
   </si>
   <si>
     <t>Arto</t>
+  </si>
+  <si>
+    <t>Use RDKit source</t>
+  </si>
+  <si>
+    <t>Name update</t>
+  </si>
+  <si>
+    <t>Weiner</t>
+  </si>
+  <si>
+    <t>Mweiner</t>
+  </si>
+  <si>
+    <t>BalabanJ</t>
+  </si>
+  <si>
+    <t>Use RDKIT source</t>
+  </si>
+  <si>
+    <t>LogTidgi</t>
+  </si>
+  <si>
+    <t>Log of the Tidgi</t>
+  </si>
+  <si>
+    <t>diameter</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>petitjean</t>
+  </si>
+  <si>
+    <t>LogGMTI</t>
   </si>
 </sst>
 </file>
@@ -1632,13 +1668,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8406698-312A-49AB-AD0D-9F939A7C75FD}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1672,6 +1713,12 @@
       <c r="B3">
         <v>6959</v>
       </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1680,6 +1727,12 @@
       <c r="B4">
         <v>7.7065340000000004</v>
       </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1688,184 +1741,285 @@
       <c r="B5">
         <v>1.0895809999999999</v>
       </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
-      <c r="B6">
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>4.7300149999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7">
-        <v>38.05415</v>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8">
-        <v>4.5194869999999998</v>
+        <v>38.05415</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9">
-        <v>68</v>
+        <v>4.5194869999999998</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10">
-        <v>95.5</v>
+      <c r="C10" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11">
-        <v>9.9727479999999993</v>
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12">
-        <v>3.2500360000000001</v>
+        <v>95.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B13">
-        <v>196.94242399999999</v>
+        <v>9.9727479999999993</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14">
-        <v>30591</v>
+        <v>3.2500360000000001</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B15">
-        <v>230</v>
+        <v>196.94242399999999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16">
+        <v>30591</v>
+      </c>
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17">
+        <v>230</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>113</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>272</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>114</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>11.805555999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>115</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>2.0293209999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>116</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>117</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>134</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>118</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>119</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>120</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>0.47368399999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C25" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>121</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>14.205446999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>122</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>2.0314960000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>123</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>2.1397309999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>124</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>2.232558</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish connectivity and start kappa
</commit_message>
<xml_diff>
--- a/doc/list_descriptor.xlsx
+++ b/doc/list_descriptor.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borrela2\development\molecular-descriptors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C082963-AE16-4B7B-95EB-422C79244F99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6051654-2CF0-4B4C-BD70-1F060F5B9DF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="-315" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13290" yWindow="2715" windowWidth="21600" windowHeight="11385" tabRatio="684" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constitution" sheetId="1" r:id="rId1"/>
     <sheet name="Molcular property" sheetId="2" r:id="rId2"/>
     <sheet name="Topological" sheetId="3" r:id="rId3"/>
     <sheet name="Connectivity" sheetId="4" r:id="rId4"/>
+    <sheet name="kappa" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="200">
   <si>
     <t>Constitutional</t>
   </si>
@@ -588,25 +589,46 @@
     <t>knotpv</t>
   </si>
   <si>
-    <t>From rdkit</t>
-  </si>
-  <si>
-    <t>Chi0n</t>
-  </si>
-  <si>
-    <t>Chi1n</t>
-  </si>
-  <si>
-    <t>Chi2n</t>
-  </si>
-  <si>
-    <t>Chi3n</t>
-  </si>
-  <si>
-    <t>Chi4n</t>
-  </si>
-  <si>
     <t>update rdkit 3.1</t>
+  </si>
+  <si>
+    <t>Keep current version</t>
+  </si>
+  <si>
+    <t>Chi0n in rdkit</t>
+  </si>
+  <si>
+    <t>Chi1n in rdkit</t>
+  </si>
+  <si>
+    <t>Chi2n in rdkit</t>
+  </si>
+  <si>
+    <t>Chi3n in rdkit</t>
+  </si>
+  <si>
+    <t>Chi4n in rdkit</t>
+  </si>
+  <si>
+    <t>kappa1</t>
+  </si>
+  <si>
+    <t>kappa2</t>
+  </si>
+  <si>
+    <t>kappa3</t>
+  </si>
+  <si>
+    <t>kappam1</t>
+  </si>
+  <si>
+    <t>kappam2</t>
+  </si>
+  <si>
+    <t>kappam3</t>
+  </si>
+  <si>
+    <t>phi</t>
   </si>
 </sst>
 </file>
@@ -2314,10 +2336,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86D9B3E-6761-4EC5-BC24-988202167197}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,7 +2386,7 @@
         <v>29.760999999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2381,7 +2403,7 @@
         <v>20.957530133630101</v>
       </c>
       <c r="F4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2516,7 +2538,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -2527,7 +2549,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>157</v>
       </c>
@@ -2538,7 +2560,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -2549,7 +2571,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>159</v>
       </c>
@@ -2560,7 +2582,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -2571,7 +2593,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -2581,8 +2603,17 @@
       <c r="C22" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>22.555605297795001</v>
+      </c>
+      <c r="E22" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -2592,8 +2623,17 @@
       <c r="C23" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>13.363072155744099</v>
+      </c>
+      <c r="E23" t="s">
+        <v>189</v>
+      </c>
+      <c r="F23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -2603,8 +2643,17 @@
       <c r="C24" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>9.6118620200536302</v>
+      </c>
+      <c r="E24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>165</v>
       </c>
@@ -2614,8 +2663,17 @@
       <c r="C25" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>6.77594411722131</v>
+      </c>
+      <c r="E25" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>166</v>
       </c>
@@ -2625,8 +2683,17 @@
       <c r="C26" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>4.6380563921149296</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>167</v>
       </c>
@@ -2637,7 +2704,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -2648,7 +2715,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -2659,7 +2726,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -2670,7 +2737,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -2681,7 +2748,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>172</v>
       </c>
@@ -2692,7 +2759,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>173</v>
       </c>
@@ -2703,7 +2770,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>174</v>
       </c>
@@ -2714,7 +2781,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -2725,7 +2792,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>176</v>
       </c>
@@ -2736,7 +2803,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -2747,7 +2814,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -2758,7 +2825,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>179</v>
       </c>
@@ -2769,7 +2836,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>180</v>
       </c>
@@ -2780,7 +2847,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -2791,7 +2858,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>182</v>
       </c>
@@ -2802,7 +2869,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>183</v>
       </c>
@@ -2813,7 +2880,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>184</v>
       </c>
@@ -2824,7 +2891,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>161</v>
       </c>
@@ -2835,7 +2902,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -2844,53 +2911,106 @@
       </c>
       <c r="C46" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>187</v>
-      </c>
-      <c r="D47">
-        <v>22.555605297795001</v>
-      </c>
-      <c r="F47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>188</v>
-      </c>
-      <c r="D48">
-        <v>13.363072155744099</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>189</v>
-      </c>
-      <c r="D49">
-        <v>9.6118620200536302</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>190</v>
-      </c>
-      <c r="D50">
-        <v>6.77594411722131</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>191</v>
-      </c>
-      <c r="D51">
-        <v>4.6380563921149296</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5669C31E-62DC-4D85-A64E-E0B4A29701C2}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3">
+        <v>32.921999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4">
+        <v>15.728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5">
+        <v>8.2959999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6">
+        <v>32.921999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7">
+        <v>15.728</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8">
+        <v>8.2959999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9">
+        <v>12.0417957209302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update autocorelation descriptors: moran, geary
</commit_message>
<xml_diff>
--- a/doc/list_descriptor.xlsx
+++ b/doc/list_descriptor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borrela2\development\molecular-descriptors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC19FAF3-8CBD-4B76-B904-5BC771A9DD74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066F5BD6-6EE9-4522-8B28-6DD19291D138}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="684" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="684" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constitution" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="basak" sheetId="7" r:id="rId7"/>
     <sheet name="Estate" sheetId="8" r:id="rId8"/>
     <sheet name="Moreau-Broto autocorrelation" sheetId="9" r:id="rId9"/>
+    <sheet name="Moran autocorrelation" sheetId="10" r:id="rId10"/>
+    <sheet name="Geary autocorelation" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="955">
   <si>
     <t>Constitutional</t>
   </si>
@@ -2676,6 +2678,228 @@
   </si>
   <si>
     <t>Correlation related to the distance to each atom equal 8 (Mass)</t>
+  </si>
+  <si>
+    <t>Volume related</t>
+  </si>
+  <si>
+    <t>electronegativity relative</t>
+  </si>
+  <si>
+    <t>polarity relative</t>
+  </si>
+  <si>
+    <t>Moran</t>
+  </si>
+  <si>
+    <t>MATSm1</t>
+  </si>
+  <si>
+    <t>MATSm2</t>
+  </si>
+  <si>
+    <t>MATSm3</t>
+  </si>
+  <si>
+    <t>MATSm4</t>
+  </si>
+  <si>
+    <t>MATSm5</t>
+  </si>
+  <si>
+    <t>MATSm6</t>
+  </si>
+  <si>
+    <t>MATSm7</t>
+  </si>
+  <si>
+    <t>MATSm8</t>
+  </si>
+  <si>
+    <t>MATSv1</t>
+  </si>
+  <si>
+    <t>MATSv2</t>
+  </si>
+  <si>
+    <t>MATSv3</t>
+  </si>
+  <si>
+    <t>MATSv4</t>
+  </si>
+  <si>
+    <t>MATSv5</t>
+  </si>
+  <si>
+    <t>MATSv6</t>
+  </si>
+  <si>
+    <t>MATSv7</t>
+  </si>
+  <si>
+    <t>MATSv8</t>
+  </si>
+  <si>
+    <t>MATSe1</t>
+  </si>
+  <si>
+    <t>MATSe2</t>
+  </si>
+  <si>
+    <t>MATSe3</t>
+  </si>
+  <si>
+    <t>MATSe4</t>
+  </si>
+  <si>
+    <t>MATSe5</t>
+  </si>
+  <si>
+    <t>MATSe6</t>
+  </si>
+  <si>
+    <t>MATSe7</t>
+  </si>
+  <si>
+    <t>MATSe8</t>
+  </si>
+  <si>
+    <t>MATSp1</t>
+  </si>
+  <si>
+    <t>MATSp2</t>
+  </si>
+  <si>
+    <t>MATSp3</t>
+  </si>
+  <si>
+    <t>MATSp4</t>
+  </si>
+  <si>
+    <t>MATSp5</t>
+  </si>
+  <si>
+    <t>MATSp6</t>
+  </si>
+  <si>
+    <t>MATSp7</t>
+  </si>
+  <si>
+    <t>MATSp8</t>
+  </si>
+  <si>
+    <t>Clean sources</t>
+  </si>
+  <si>
+    <t>mass based</t>
+  </si>
+  <si>
+    <t>Volume based</t>
+  </si>
+  <si>
+    <t>Electro based</t>
+  </si>
+  <si>
+    <t>Polaribility based</t>
+  </si>
+  <si>
+    <t>GATSm1</t>
+  </si>
+  <si>
+    <t>GATSm2</t>
+  </si>
+  <si>
+    <t>GATSm3</t>
+  </si>
+  <si>
+    <t>GATSm4</t>
+  </si>
+  <si>
+    <t>GATSm5</t>
+  </si>
+  <si>
+    <t>GATSm6</t>
+  </si>
+  <si>
+    <t>GATSm7</t>
+  </si>
+  <si>
+    <t>GATSm8</t>
+  </si>
+  <si>
+    <t>GATSv1</t>
+  </si>
+  <si>
+    <t>GATSv2</t>
+  </si>
+  <si>
+    <t>GATSv3</t>
+  </si>
+  <si>
+    <t>GATSv4</t>
+  </si>
+  <si>
+    <t>GATSv5</t>
+  </si>
+  <si>
+    <t>GATSv6</t>
+  </si>
+  <si>
+    <t>GATSv7</t>
+  </si>
+  <si>
+    <t>GATSv8</t>
+  </si>
+  <si>
+    <t>GATSe1</t>
+  </si>
+  <si>
+    <t>GATSe2</t>
+  </si>
+  <si>
+    <t>GATSe3</t>
+  </si>
+  <si>
+    <t>GATSe4</t>
+  </si>
+  <si>
+    <t>GATSe5</t>
+  </si>
+  <si>
+    <t>GATSe6</t>
+  </si>
+  <si>
+    <t>GATSe7</t>
+  </si>
+  <si>
+    <t>GATSe8</t>
+  </si>
+  <si>
+    <t>GATSp1</t>
+  </si>
+  <si>
+    <t>GATSp2</t>
+  </si>
+  <si>
+    <t>GATSp3</t>
+  </si>
+  <si>
+    <t>GATSp4</t>
+  </si>
+  <si>
+    <t>GATSp5</t>
+  </si>
+  <si>
+    <t>GATSp6</t>
+  </si>
+  <si>
+    <t>GATSp7</t>
+  </si>
+  <si>
+    <t>GATSp8</t>
+  </si>
+  <si>
+    <t>Geary</t>
   </si>
 </sst>
 </file>
@@ -3715,6 +3939,1014 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B1A4C5-DD22-4302-AD1C-8537DC117209}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>885</v>
+      </c>
+      <c r="B3">
+        <v>-0.15774299999999999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>885</v>
+      </c>
+      <c r="D3">
+        <v>-0.15774299999999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>918</v>
+      </c>
+      <c r="F3" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>886</v>
+      </c>
+      <c r="B4">
+        <v>0.168709</v>
+      </c>
+      <c r="C4" t="s">
+        <v>886</v>
+      </c>
+      <c r="D4">
+        <v>0.168709</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>887</v>
+      </c>
+      <c r="B5">
+        <v>-0.145481</v>
+      </c>
+      <c r="C5" t="s">
+        <v>887</v>
+      </c>
+      <c r="D5">
+        <v>-0.145481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>888</v>
+      </c>
+      <c r="B6">
+        <v>-1.7170999999999999E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>888</v>
+      </c>
+      <c r="D6">
+        <v>-1.7170999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>889</v>
+      </c>
+      <c r="B7">
+        <v>-0.16705200000000001</v>
+      </c>
+      <c r="C7" t="s">
+        <v>889</v>
+      </c>
+      <c r="D7">
+        <v>-0.16705200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>890</v>
+      </c>
+      <c r="B8">
+        <v>0.22050800000000001</v>
+      </c>
+      <c r="C8" t="s">
+        <v>890</v>
+      </c>
+      <c r="D8">
+        <v>0.22050800000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>891</v>
+      </c>
+      <c r="B9">
+        <v>-0.223131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>891</v>
+      </c>
+      <c r="D9">
+        <v>-0.223131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>892</v>
+      </c>
+      <c r="B10">
+        <v>3.2912999999999998E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>892</v>
+      </c>
+      <c r="D10">
+        <v>3.2912999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>893</v>
+      </c>
+      <c r="B11">
+        <v>-0.17894299999999999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>893</v>
+      </c>
+      <c r="D11">
+        <v>-0.17894299999999999</v>
+      </c>
+      <c r="E11" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>894</v>
+      </c>
+      <c r="B12">
+        <v>0.20768</v>
+      </c>
+      <c r="C12" t="s">
+        <v>894</v>
+      </c>
+      <c r="D12">
+        <v>0.20768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>895</v>
+      </c>
+      <c r="B13">
+        <v>-0.15917100000000001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>895</v>
+      </c>
+      <c r="D13">
+        <v>-0.15917100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>896</v>
+      </c>
+      <c r="B14">
+        <v>3.2120999999999997E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>896</v>
+      </c>
+      <c r="D14">
+        <v>3.2120999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>897</v>
+      </c>
+      <c r="B15">
+        <v>-0.18659899999999999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>897</v>
+      </c>
+      <c r="D15">
+        <v>-0.18659899999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>898</v>
+      </c>
+      <c r="B16">
+        <v>0.219303</v>
+      </c>
+      <c r="C16" t="s">
+        <v>898</v>
+      </c>
+      <c r="D16">
+        <v>0.219303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>899</v>
+      </c>
+      <c r="B17">
+        <v>-0.21523600000000001</v>
+      </c>
+      <c r="C17" t="s">
+        <v>899</v>
+      </c>
+      <c r="D17">
+        <v>-0.21523600000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>900</v>
+      </c>
+      <c r="B18">
+        <v>2.2724000000000001E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>900</v>
+      </c>
+      <c r="D18">
+        <v>2.2724000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>901</v>
+      </c>
+      <c r="B19">
+        <v>-0.15543299999999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>901</v>
+      </c>
+      <c r="D19">
+        <v>-0.15543299999999999</v>
+      </c>
+      <c r="E19" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>902</v>
+      </c>
+      <c r="B20">
+        <v>0.16495599999999999</v>
+      </c>
+      <c r="C20" t="s">
+        <v>902</v>
+      </c>
+      <c r="D20">
+        <v>0.16495599999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>903</v>
+      </c>
+      <c r="B21">
+        <v>-0.143733</v>
+      </c>
+      <c r="C21" t="s">
+        <v>903</v>
+      </c>
+      <c r="D21">
+        <v>-0.143733</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>904</v>
+      </c>
+      <c r="B22">
+        <v>-2.2377999999999999E-2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>904</v>
+      </c>
+      <c r="D22">
+        <v>-2.2377999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>905</v>
+      </c>
+      <c r="B23">
+        <v>-0.164774</v>
+      </c>
+      <c r="C23" t="s">
+        <v>905</v>
+      </c>
+      <c r="D23">
+        <v>-0.164774</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>906</v>
+      </c>
+      <c r="B24">
+        <v>0.220165</v>
+      </c>
+      <c r="C24" t="s">
+        <v>906</v>
+      </c>
+      <c r="D24">
+        <v>0.220165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>907</v>
+      </c>
+      <c r="B25">
+        <v>-0.22389500000000001</v>
+      </c>
+      <c r="C25" t="s">
+        <v>907</v>
+      </c>
+      <c r="D25">
+        <v>-0.22389500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>908</v>
+      </c>
+      <c r="B26">
+        <v>3.3782E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>908</v>
+      </c>
+      <c r="D26">
+        <v>3.3782E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>909</v>
+      </c>
+      <c r="B27">
+        <v>-0.18820700000000001</v>
+      </c>
+      <c r="C27" t="s">
+        <v>909</v>
+      </c>
+      <c r="D27">
+        <v>-0.18820700000000001</v>
+      </c>
+      <c r="E27" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>910</v>
+      </c>
+      <c r="B28">
+        <v>0.22777</v>
+      </c>
+      <c r="C28" t="s">
+        <v>910</v>
+      </c>
+      <c r="D28">
+        <v>0.22777</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>911</v>
+      </c>
+      <c r="B29">
+        <v>-0.16356299999999999</v>
+      </c>
+      <c r="C29" t="s">
+        <v>911</v>
+      </c>
+      <c r="D29">
+        <v>-0.16356299999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>912</v>
+      </c>
+      <c r="B30">
+        <v>5.4676000000000002E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>912</v>
+      </c>
+      <c r="D30">
+        <v>5.4676000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>913</v>
+      </c>
+      <c r="B31">
+        <v>-0.194218</v>
+      </c>
+      <c r="C31" t="s">
+        <v>913</v>
+      </c>
+      <c r="D31">
+        <v>-0.194218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>914</v>
+      </c>
+      <c r="B32">
+        <v>0.215838</v>
+      </c>
+      <c r="C32" t="s">
+        <v>914</v>
+      </c>
+      <c r="D32">
+        <v>0.215838</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>915</v>
+      </c>
+      <c r="B33">
+        <v>-0.21119099999999999</v>
+      </c>
+      <c r="C33" t="s">
+        <v>915</v>
+      </c>
+      <c r="D33">
+        <v>-0.21119099999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>916</v>
+      </c>
+      <c r="B34">
+        <v>1.6775999999999999E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>916</v>
+      </c>
+      <c r="D34">
+        <v>1.6775999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EE91B9-2151-4DED-8739-892DB78E1E96}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>922</v>
+      </c>
+      <c r="B3">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="C3" t="s">
+        <v>922</v>
+      </c>
+      <c r="D3">
+        <v>0.90730599999999995</v>
+      </c>
+      <c r="F3" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>923</v>
+      </c>
+      <c r="B4">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="C4" t="s">
+        <v>923</v>
+      </c>
+      <c r="D4">
+        <v>0.73868400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>924</v>
+      </c>
+      <c r="B5">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>924</v>
+      </c>
+      <c r="D5">
+        <v>1.205133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>925</v>
+      </c>
+      <c r="B6">
+        <v>1.234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>925</v>
+      </c>
+      <c r="D6">
+        <v>1.233719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>926</v>
+      </c>
+      <c r="B7">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>926</v>
+      </c>
+      <c r="D7">
+        <v>1.267058</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>927</v>
+      </c>
+      <c r="B8">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="C8" t="s">
+        <v>927</v>
+      </c>
+      <c r="D8">
+        <v>0.92865600000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>928</v>
+      </c>
+      <c r="B9">
+        <v>1.274</v>
+      </c>
+      <c r="C9" t="s">
+        <v>928</v>
+      </c>
+      <c r="D9">
+        <v>1.2741130000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>929</v>
+      </c>
+      <c r="B10">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>929</v>
+      </c>
+      <c r="D10">
+        <v>1.066859</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>930</v>
+      </c>
+      <c r="B11">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="C11" t="s">
+        <v>930</v>
+      </c>
+      <c r="D11">
+        <v>0.95217600000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>931</v>
+      </c>
+      <c r="B12">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="C12" t="s">
+        <v>931</v>
+      </c>
+      <c r="D12">
+        <v>0.72316000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B13">
+        <v>1.222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>932</v>
+      </c>
+      <c r="D13">
+        <v>1.2223109999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>933</v>
+      </c>
+      <c r="B14">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>933</v>
+      </c>
+      <c r="D14">
+        <v>1.181899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>934</v>
+      </c>
+      <c r="B15">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>934</v>
+      </c>
+      <c r="D15">
+        <v>1.2791939999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>935</v>
+      </c>
+      <c r="B16">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="C16" t="s">
+        <v>935</v>
+      </c>
+      <c r="D16">
+        <v>0.91820199999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>936</v>
+      </c>
+      <c r="B17">
+        <v>1.262</v>
+      </c>
+      <c r="C17" t="s">
+        <v>936</v>
+      </c>
+      <c r="D17">
+        <v>1.262122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>937</v>
+      </c>
+      <c r="B18">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="C18" t="s">
+        <v>937</v>
+      </c>
+      <c r="D18">
+        <v>1.0669919999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>938</v>
+      </c>
+      <c r="B19">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="C19" t="s">
+        <v>938</v>
+      </c>
+      <c r="D19">
+        <v>0.90271500000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>939</v>
+      </c>
+      <c r="B20">
+        <v>0.74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>939</v>
+      </c>
+      <c r="D20">
+        <v>0.740313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>940</v>
+      </c>
+      <c r="B21">
+        <v>1.2030000000000001</v>
+      </c>
+      <c r="C21" t="s">
+        <v>940</v>
+      </c>
+      <c r="D21">
+        <v>1.2031849999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>941</v>
+      </c>
+      <c r="B22">
+        <v>1.2390000000000001</v>
+      </c>
+      <c r="C22" t="s">
+        <v>941</v>
+      </c>
+      <c r="D22">
+        <v>1.2393749999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>942</v>
+      </c>
+      <c r="B23">
+        <v>1.266</v>
+      </c>
+      <c r="C23" t="s">
+        <v>942</v>
+      </c>
+      <c r="D23">
+        <v>1.265571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>943</v>
+      </c>
+      <c r="B24">
+        <v>0.93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>943</v>
+      </c>
+      <c r="D24">
+        <v>0.93017700000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>944</v>
+      </c>
+      <c r="B25">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="C25" t="s">
+        <v>944</v>
+      </c>
+      <c r="D25">
+        <v>1.275315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>945</v>
+      </c>
+      <c r="B26">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="C26" t="s">
+        <v>945</v>
+      </c>
+      <c r="D26">
+        <v>1.0669919999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>946</v>
+      </c>
+      <c r="B27">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="C27" t="s">
+        <v>946</v>
+      </c>
+      <c r="D27">
+        <v>0.97363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>947</v>
+      </c>
+      <c r="B28">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="C28" t="s">
+        <v>947</v>
+      </c>
+      <c r="D28">
+        <v>0.71599000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>948</v>
+      </c>
+      <c r="B29">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="C29" t="s">
+        <v>948</v>
+      </c>
+      <c r="D29">
+        <v>1.229346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>949</v>
+      </c>
+      <c r="B30">
+        <v>1.159</v>
+      </c>
+      <c r="C30" t="s">
+        <v>949</v>
+      </c>
+      <c r="D30">
+        <v>1.1593249999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>950</v>
+      </c>
+      <c r="B31">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="C31" t="s">
+        <v>950</v>
+      </c>
+      <c r="D31">
+        <v>1.2834719999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>951</v>
+      </c>
+      <c r="B32">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="C32" t="s">
+        <v>951</v>
+      </c>
+      <c r="D32">
+        <v>0.91600400000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>952</v>
+      </c>
+      <c r="B33">
+        <v>1.256</v>
+      </c>
+      <c r="C33" t="s">
+        <v>952</v>
+      </c>
+      <c r="D33">
+        <v>1.2562340000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>953</v>
+      </c>
+      <c r="B34">
+        <v>1.0680000000000001</v>
+      </c>
+      <c r="C34" t="s">
+        <v>953</v>
+      </c>
+      <c r="D34">
+        <v>1.0679650000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F12"/>
@@ -10620,8 +11852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4283E985-4A18-4525-904E-F38821CBAA2F}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10831,6 +12063,9 @@
       <c r="D11">
         <v>3.7077429999999998</v>
       </c>
+      <c r="E11" t="s">
+        <v>881</v>
+      </c>
       <c r="F11" t="s">
         <v>878</v>
       </c>
@@ -10967,6 +12202,9 @@
       <c r="D19">
         <v>3.9895900000000002</v>
       </c>
+      <c r="E19" t="s">
+        <v>882</v>
+      </c>
       <c r="F19" t="s">
         <v>878</v>
       </c>
@@ -11102,6 +12340,9 @@
       </c>
       <c r="D27">
         <v>3.6742849999999998</v>
+      </c>
+      <c r="E27" t="s">
+        <v>883</v>
       </c>
       <c r="F27" t="s">
         <v>878</v>

</xml_diff>